<commit_message>
finished read_excel in construction dataset class. Many other modification to materials and windows
</commit_message>
<xml_diff>
--- a/eureca_building/example_scripts/materials_and_construction_test.xlsx
+++ b/eureca_building/example_scripts/materials_and_construction_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr15640\Desktop\EUReCA-building\eureca_building\example_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172B9265-5DBB-4D49-BE6D-7EC671D204E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35A1E51-140C-41A5-ABFC-69826605F6E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="228" windowWidth="17988" windowHeight="10440" tabRatio="823" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="114">
   <si>
     <t>id</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Window</t>
   </si>
   <si>
-    <t>opaque_type_name</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -385,9 +382,6 @@
     <t>frame_factor [-]</t>
   </si>
   <si>
-    <t>shading_coeff_int [-]</t>
-  </si>
-  <si>
     <t>shading_coef_ext [-]</t>
   </si>
   <si>
@@ -416,6 +410,9 @@
   </si>
   <si>
     <t>AirGapMaterial</t>
+  </si>
+  <si>
+    <t>shading_coef_int [-]</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
@@ -1047,10 +1044,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="8">
         <v>13</v>
@@ -1086,10 +1083,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="8">
         <v>34</v>
@@ -1125,10 +1122,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="8">
         <v>55</v>
@@ -1273,7 +1270,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1327,8 +1324,8 @@
   <dimension ref="A1:AMI33"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1353,37 +1350,37 @@
         <v>8</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -1391,13 +1388,13 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1">
         <v>20</v>
@@ -1426,13 +1423,13 @@
         <v>14</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1">
         <v>3</v>
@@ -1459,13 +1456,13 @@
         <v>15</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -1488,13 +1485,13 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1">
         <v>6</v>
@@ -1519,13 +1516,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1">
         <v>12</v>
@@ -1554,13 +1551,13 @@
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1">
         <v>14</v>
@@ -1583,13 +1580,13 @@
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
@@ -1618,13 +1615,13 @@
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1">
         <v>40</v>
@@ -1657,13 +1654,13 @@
         <v>35</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1">
         <v>3</v>
@@ -1690,13 +1687,13 @@
         <v>36</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1">
         <v>3</v>
@@ -1723,13 +1720,13 @@
         <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1">
         <v>6</v>
@@ -1754,13 +1751,13 @@
         <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1">
         <v>12</v>
@@ -1791,13 +1788,13 @@
         <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="1">
         <v>14</v>
@@ -1820,13 +1817,13 @@
         <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
@@ -1853,13 +1850,13 @@
         <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="1">
         <v>6</v>
@@ -1886,13 +1883,13 @@
         <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1">
         <v>12</v>
@@ -1925,13 +1922,13 @@
         <v>53</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1">
         <v>14</v>
@@ -1954,13 +1951,13 @@
         <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -1993,13 +1990,13 @@
         <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1">
         <v>40</v>
@@ -2032,13 +2029,13 @@
         <v>56</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -2063,13 +2060,13 @@
         <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="1">
         <v>6</v>
@@ -2096,13 +2093,13 @@
         <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1">
         <v>12</v>
@@ -2135,13 +2132,13 @@
         <v>59</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E24" s="1">
         <v>14</v>
@@ -2164,13 +2161,13 @@
         <v>60</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E25" s="1">
         <v>3</v>
@@ -2203,13 +2200,13 @@
         <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26" s="1">
         <v>40</v>
@@ -2250,13 +2247,13 @@
         <v>62</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" s="1">
         <v>3</v>
@@ -2385,8 +2382,8 @@
   <dimension ref="A1:AMI163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2409,25 +2406,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>112</v>
       </c>
       <c r="K1" s="1"/>
       <c r="AMG1" s="7"/>
@@ -2439,10 +2436,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1">
         <v>0.03</v>
@@ -2466,10 +2463,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1">
         <v>1.4999999999999999E-2</v>
@@ -2494,10 +2491,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7">
         <v>0.02</v>
@@ -2521,10 +2518,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7">
         <v>0.02</v>
@@ -2548,10 +2545,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1">
         <v>0.4</v>
@@ -2575,10 +2572,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1">
         <v>0.3</v>
@@ -2602,10 +2599,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7">
         <v>0.1</v>
@@ -2629,10 +2626,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1">
         <v>0.02</v>
@@ -2656,10 +2653,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1">
         <v>0.2</v>
@@ -2683,10 +2680,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1">
         <v>0.06</v>
@@ -2710,10 +2707,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1">
         <v>0.01</v>
@@ -2737,10 +2734,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1">
         <v>1.4999999999999999E-2</v>
@@ -2764,10 +2761,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="7">
         <v>0.06</v>
@@ -2791,10 +2788,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="7">
         <v>1.4999999999999999E-2</v>
@@ -2818,10 +2815,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="1">
         <v>0.375</v>
@@ -2845,10 +2842,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1">
         <v>0.16</v>
@@ -2872,10 +2869,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1">
         <v>0.04</v>
@@ -2899,10 +2896,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1">
         <v>0.03</v>
@@ -2926,10 +2923,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="7">
         <v>0.12</v>
@@ -2953,10 +2950,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1">
         <v>0.01</v>
@@ -2980,10 +2977,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1">
         <v>0.08</v>
@@ -3007,10 +3004,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D23" s="22">
         <v>0.05</v>
@@ -4047,10 +4044,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="1">
         <v>0.25</v>
@@ -4074,10 +4071,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" s="1">
         <v>0.3</v>
@@ -4101,10 +4098,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" s="7">
         <v>0.08</v>
@@ -4128,10 +4125,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1">
         <v>0.02</v>
@@ -4155,10 +4152,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" s="7">
         <v>0.06</v>
@@ -4182,10 +4179,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29" s="1">
         <v>0.16</v>
@@ -4209,10 +4206,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30" s="1">
         <v>0.15</v>
@@ -4236,10 +4233,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D31" s="27">
         <v>0.08</v>
@@ -5276,10 +5273,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D32" s="7">
         <v>0.12</v>
@@ -5303,10 +5300,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D33" s="27">
         <v>0.06</v>
@@ -6343,10 +6340,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34" s="7">
         <v>0.06</v>
@@ -6370,10 +6367,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D35" s="7">
         <v>0.25</v>
@@ -6397,10 +6394,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D36" s="27">
         <v>0.02</v>
@@ -7436,10 +7433,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" s="7">
         <v>0.25</v>
@@ -7463,10 +7460,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D38" s="7">
         <v>0.03</v>
@@ -7490,10 +7487,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D39" s="7">
         <v>0.01</v>
@@ -7517,10 +7514,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D40" s="7">
         <v>0.12</v>
@@ -7544,10 +7541,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D41" s="7">
         <v>0.03</v>
@@ -7571,10 +7568,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D42" s="7">
         <v>0.02</v>
@@ -7598,10 +7595,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D43" s="7">
         <v>0.06</v>
@@ -7625,10 +7622,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D44" s="1">
         <v>0.24</v>
@@ -7652,10 +7649,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D45" s="7">
         <v>0.25</v>
@@ -7679,10 +7676,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D46" s="7">
         <v>0.04</v>
@@ -7706,10 +7703,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D47" s="7">
         <v>0.12</v>
@@ -7733,10 +7730,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D48" s="7">
         <v>0.05</v>
@@ -7760,10 +7757,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D49" s="7">
         <v>0.38</v>
@@ -7787,10 +7784,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D50" s="7">
         <v>0.1</v>
@@ -7814,10 +7811,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D51" s="7">
         <v>0.16</v>
@@ -7841,10 +7838,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D52" s="7">
         <v>0.3</v>
@@ -7868,10 +7865,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D53" s="7">
         <v>0.15</v>
@@ -7895,10 +7892,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D54" s="1">
         <v>0.3</v>
@@ -7922,10 +7919,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D55" s="27">
         <v>0.04</v>
@@ -9246,22 +9243,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -9269,7 +9266,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3">
         <v>4.9000000000000004</v>
@@ -9295,7 +9292,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2">
         <v>3.7</v>
@@ -9321,7 +9318,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2">
         <v>2.2000000000000002</v>
@@ -9361,6 +9358,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B4A72D35825A314C9EB5C5BDD49EC582" ma:contentTypeVersion="10" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ab3cfd4ffe88710ffd03436b1addd592">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c0574b82-72ca-428d-96cb-9dbc44012ede" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb55e547d0e393e34c6bbb534eb78df0" ns3:_="">
     <xsd:import namespace="c0574b82-72ca-428d-96cb-9dbc44012ede"/>
@@ -9544,35 +9556,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81EF3F0-7775-4285-BFE0-18A3A29E794A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8F108CF-CFD9-47FB-AD65-C74A1CC8D454}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c0574b82-72ca-428d-96cb-9dbc44012ede"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9594,9 +9581,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8F108CF-CFD9-47FB-AD65-C74A1CC8D454}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81EF3F0-7775-4285-BFE0-18A3A29E794A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c0574b82-72ca-428d-96cb-9dbc44012ede"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>